<commit_message>
Added R26/R27 Pulldowns on LED pins from arduino
</commit_message>
<xml_diff>
--- a/ww101-shield/eagle/ww101board.xlsx
+++ b/ww101-shield/eagle/ww101board.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9100" yWindow="5060" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="21220" yWindow="5540" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ww101board" localSheetId="0">Sheet1!$A$1:$E$61</definedName>
+    <definedName name="ww101board" localSheetId="0">Sheet1!$A$1:$E$63</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +32,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="ww101board" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/arh/Documents/iotexpert-projects/WA101/ww101-shield/eagle/ww101board.csv" tab="0" semicolon="1">
+    <textPr fileType="mac" sourceFile="/Users/arh/Documents/iotexpert-projects/WA101/ww101-shield/eagle/ww101board.csv" tab="0" semicolon="1">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="115">
   <si>
     <t>Part</t>
   </si>
@@ -385,6 +385,15 @@
   </si>
   <si>
     <t>10K Thermister</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>50K</t>
   </si>
 </sst>
 </file>
@@ -736,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1710,7 +1719,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>97</v>
@@ -1719,57 +1728,91 @@
         <v>64</v>
       </c>
       <c r="D58" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="E58" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="C59" t="s">
         <v>64</v>
       </c>
       <c r="D59" t="s">
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="E59" t="s">
-        <v>104</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="C60" t="s">
         <v>64</v>
       </c>
       <c r="D60" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E60" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>102</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C61" t="s">
+        <v>64</v>
+      </c>
+      <c r="D61" t="s">
+        <v>103</v>
+      </c>
+      <c r="E61" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>105</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" t="s">
+        <v>64</v>
+      </c>
+      <c r="D62" t="s">
+        <v>106</v>
+      </c>
+      <c r="E62" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>107</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C63" t="s">
         <v>108</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D63" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>